<commit_message>
PIO files added and white code added to xlsx file
</commit_message>
<xml_diff>
--- a/IRcodes.xlsx
+++ b/IRcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d451e8338758ec2/Escritorio/Programas/ESP8266-IR2WiFiHack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{46EE5801-5E17-4272-9E82-A51DAC1BD8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{272B5F4F-E777-4695-8FCB-9513E70A3C24}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{46EE5801-5E17-4272-9E82-A51DAC1BD8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3AAF15C0-4185-4791-9ADD-B2AA7AF3BC92}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B82338D5-7CAF-40AA-BD78-04BF3F5614BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
   <si>
     <t>Function</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Sky blue</t>
   </si>
   <si>
-    <t>Lime</t>
-  </si>
-  <si>
     <t>Violet</t>
   </si>
   <si>
@@ -178,13 +175,70 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Light Green</t>
+  </si>
+  <si>
+    <t>NO USAR</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>0x00F720DFUL</t>
+  </si>
+  <si>
+    <t>0x00F710EFUL</t>
+  </si>
+  <si>
+    <t>0x00F728D7UL</t>
+  </si>
+  <si>
+    <t>0x00F730CFUL</t>
+  </si>
+  <si>
+    <t>0x00F78877UL</t>
+  </si>
+  <si>
+    <t>0x00F7906FUL</t>
+  </si>
+  <si>
+    <t>0x00F7B04FUL</t>
+  </si>
+  <si>
+    <t>0x00F76897UL</t>
+  </si>
+  <si>
+    <t>0x00F7A05FUL</t>
+  </si>
+  <si>
+    <t>0x00F7708FUL</t>
+  </si>
+  <si>
+    <t>0x00F750AFUL</t>
+  </si>
+  <si>
+    <t>0x00F7609FUL</t>
+  </si>
+  <si>
+    <t>0x00F748B7UL</t>
+  </si>
+  <si>
+    <t>0x00F7A857UL</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>0x00F7E01FUL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,8 +252,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +357,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -309,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -328,6 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,16 +724,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B30C858-E331-454D-82B5-45903F726972}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -682,15 +751,17 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="J1" s="17"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -729,8 +800,7 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="17">
-        <f>(F2*(G2*10)*H2)</f>
+      <c r="I2" s="16">
         <v>0</v>
       </c>
       <c r="J2" s="16"/>
@@ -747,7 +817,6 @@
       <c r="U2" s="16"/>
       <c r="V2" s="16"/>
       <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -757,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>19</v>
@@ -772,8 +841,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="16">
-        <f>(F3*(G3*10)*H3)</f>
-        <v>22.400000000000002</v>
+        <v>2</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
@@ -789,7 +857,6 @@
       <c r="U3" s="16"/>
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -814,8 +881,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="16">
-        <f>(F4*(G4*10))</f>
-        <v>298</v>
+        <v>29</v>
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
@@ -831,7 +897,6 @@
       <c r="U4" s="16"/>
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -841,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>15</v>
@@ -856,8 +921,7 @@
         <v>0.9</v>
       </c>
       <c r="I5" s="16">
-        <f>(F5*(G5*10)*H5)</f>
-        <v>204.3</v>
+        <v>25</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
@@ -873,7 +937,6 @@
       <c r="U5" s="16"/>
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -892,8 +955,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f>(F6*(G6*10))</f>
-        <v>600</v>
+        <v>60</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
@@ -909,7 +971,6 @@
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -934,8 +995,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="16">
-        <f>(F7*(G7*10))</f>
-        <v>1200</v>
+        <v>120</v>
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
@@ -951,7 +1011,6 @@
       <c r="U7" s="16"/>
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -961,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>33</v>
@@ -976,8 +1035,7 @@
         <v>0.9</v>
       </c>
       <c r="I8" s="16">
-        <f>(F8*(G8*10)*H8)</f>
-        <v>432</v>
+        <v>44</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
@@ -993,7 +1051,6 @@
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
       <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1009,17 +1066,16 @@
         <v>17</v>
       </c>
       <c r="F9">
-        <v>192</v>
+        <v>197.4</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0.43</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="I9" s="16">
-        <f>(F9*(G9*10)*H9)</f>
-        <v>1920</v>
+        <v>77</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
@@ -1035,7 +1091,6 @@
       <c r="U9" s="16"/>
       <c r="V9" s="16"/>
       <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
@@ -1054,8 +1109,7 @@
         <v>0.9</v>
       </c>
       <c r="I10" s="16">
-        <f>(F10*(G10*10)*H10)</f>
-        <v>349.2</v>
+        <v>43</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
@@ -1071,11 +1125,10 @@
       <c r="U10" s="16"/>
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>27</v>
@@ -1089,9 +1142,8 @@
       <c r="H11">
         <v>0.5</v>
       </c>
-      <c r="I11" s="16">
-        <f>(F11*(G11*10)*H11)</f>
-        <v>1200</v>
+      <c r="I11" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
@@ -1107,7 +1159,6 @@
       <c r="U11" s="16"/>
       <c r="V11" s="16"/>
       <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
@@ -1126,8 +1177,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="16">
-        <f>(F12*(G12*10))</f>
-        <v>2400</v>
+        <v>240</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
@@ -1143,11 +1193,10 @@
       <c r="U12" s="16"/>
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>30</v>
@@ -1162,8 +1211,7 @@
         <v>0.8</v>
       </c>
       <c r="I13" s="16">
-        <f>(F13*(G13*10)*H13)</f>
-        <v>2256</v>
+        <v>233</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
@@ -1179,11 +1227,10 @@
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>31</v>
@@ -1198,8 +1245,7 @@
         <v>0.8</v>
       </c>
       <c r="I14" s="16">
-        <f>(F14*(G14*10)*H14)</f>
-        <v>1735.0400000000002</v>
+        <v>194</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
@@ -1215,11 +1261,10 @@
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
       <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>32</v>
@@ -1234,8 +1279,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="16">
-        <f>(F15*(G15*10))</f>
-        <v>2698</v>
+        <v>269</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
@@ -1251,11 +1295,10 @@
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
       <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>18</v>
@@ -1270,8 +1313,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="16">
-        <f>(F16*(G16*10))</f>
-        <v>873.75</v>
+        <v>86</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
@@ -1287,7 +1329,6 @@
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
       <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
     </row>
     <row r="17" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
@@ -1332,7 +1373,24 @@
       <c r="X18" s="16"/>
     </row>
     <row r="19" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I19" s="16"/>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -1350,7 +1408,24 @@
       <c r="X19" s="16"/>
     </row>
     <row r="20" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I20" s="16"/>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0</v>
+      </c>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
@@ -1368,7 +1443,24 @@
       <c r="X20" s="16"/>
     </row>
     <row r="21" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I21" s="16"/>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21">
+        <v>3.2</v>
+      </c>
+      <c r="G21">
+        <v>0.7</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="16">
+        <v>2</v>
+      </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
@@ -1386,7 +1478,25 @@
       <c r="X21" s="16"/>
     </row>
     <row r="22" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I22" s="16"/>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <v>35.85</v>
+      </c>
+      <c r="G22">
+        <v>0.32</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f>ROUND(F22*G22,0)</f>
+        <v>11</v>
+      </c>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
@@ -1403,7 +1513,270 @@
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
     </row>
+    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23">
+        <v>45.4</v>
+      </c>
+      <c r="G23">
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <v>0.9</v>
+      </c>
+      <c r="I23" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24">
+        <v>29.8</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" s="16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25">
+        <v>194</v>
+      </c>
+      <c r="G25">
+        <v>0.2</v>
+      </c>
+      <c r="H25">
+        <v>0.9</v>
+      </c>
+      <c r="I25" s="16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26">
+        <v>120</v>
+      </c>
+      <c r="G26">
+        <v>0.4</v>
+      </c>
+      <c r="H26">
+        <v>0.9</v>
+      </c>
+      <c r="I26" s="16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27">
+        <v>60</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28">
+        <v>197.4</v>
+      </c>
+      <c r="G28">
+        <v>0.43</v>
+      </c>
+      <c r="H28">
+        <v>0.92</v>
+      </c>
+      <c r="I28" s="16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>349.5</v>
+      </c>
+      <c r="G29">
+        <v>0.25</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>120</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30" s="16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31">
+        <v>271.10000000000002</v>
+      </c>
+      <c r="G31">
+        <v>0.8</v>
+      </c>
+      <c r="H31">
+        <v>0.8</v>
+      </c>
+      <c r="I31" s="16">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32">
+        <v>282</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0.8</v>
+      </c>
+      <c r="I32" s="16">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33">
+        <v>240</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" s="16">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>269.8</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" s="16">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35">
+        <v>240</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0.5</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D21:I35">
+    <sortCondition ref="I35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>